<commit_message>
First two steps of second stage completed
</commit_message>
<xml_diff>
--- a/All Records with 2digit filters.xlsx
+++ b/All Records with 2digit filters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <x:si>
     <x:t>Site Name</x:t>
   </x:si>
@@ -31,335 +31,351 @@
     <x:t>Filter dashes</x:t>
   </x:si>
   <x:si>
-    <x:t>U.S. Government seeks to lease 7,400 - 8,000 ABOA SF of Office and Related Space in Bemidji, MN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/ba90a73e3ebe43469df1c7d541ef77d4/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>U.S. Government seeks to lease 7,400 - 8,000 ABOA SF of Office and Related Space in Bemidji, MN
-Notice ID: 1MN2107
-General Services Administration (GSA) seeks to lease the following space:
-State: Minnesota
-City:
+    <x:t>Small Tactical Electric Power 3-Kilowatt(STEP 3kW)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sam.gov/opp/89685cb08be14b2d9664b0cd90055f26/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Small Tactical Electric Power 3-Kilowatt(STEP 3kW)
+Notice ID: W909MY-22-R-0009
+Introduction
+This Solicitation is for the award of up to three (3) Engineering and Manufacturing Development (EMD) contracts for a new/improv
 ...
 Department/Ind.Agency
-GENERAL SERVICES ADMINISTRATION
-Subtier
-PUBLIC BUILDINGS SERVICE
-Office
-PBS R5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Contract Opportunities
-Current Date Offers Due
-July 23, 2022, 05:59 AM GMT+1
-Notice Type
-Original Combined Synopsis/Solicitation
-Updated Date
-Jun 7, 2022
-Published Date
-Jun 7, 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>X1DB--Port Charlotte CBOC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/e9f3b667e8b14c878166f66afaa662c4/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>X1DB--Port Charlotte CBOC
-Notice ID: 36C24822R0048
-The purpose of this amendment is to: Extend the due date for responses Respond to questions and answers (see attached Questions and Answers pdf) ...
+DEPT OF DEFENSE
+Subtier
+DEPT OF THE ARMY
+Office
+ACC-ABERDEEN PROVING GROUNDS CONT C</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract Opportunities
+Current Date Offers Due
+July 25, 2022, 07:00 PM GMT+1
+Notice Type
+Original Solicitation
+Updated Date
+Jun 10, 2022
+Published Date
+Jun 10, 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Repair of C-5 Tubing and Fitting (Aileron Servo Assembly)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sam.gov/opp/27e92b1e2ac04a1791f1811b796c9133/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Repair of C-5 Tubing and Fitting (Aileron Servo Assembly)
+Notice ID: FA853822R0013
+This notice is the formal issuance of Solicitation FA8538-22-R-0013 issued by AFSC/PZAAB C-5, C-130, and F-15 Supply Chain Contracting Section. The
+...
+Department/Ind.Agency
+DEPT OF DEFENSE
+Subtier
+DEPT OF THE AIR FORCE
+Office
+FA8538 AFSC PZAAB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract Opportunities
+Current Date Offers Due
+July 25, 2022, 09:00 PM GMT+1
+Notice Type
+Original Solicitation
+Updated Date
+Jun 10, 2022
+Published Date
+Jun 10, 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Y1DA--652-18-930 ER Headwall Renovation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sam.gov/opp/cbcb935cace6426c94559cf5400f6252/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Y1DA--652-18-930 ER Headwall Renovation
+Notice ID: 36C24622B0010
+See SOW for Additional Information ...
 Department/Ind.Agency
 VETERANS AFFAIRS, DEPARTMENT OF
 Subtier
 VETERANS AFFAIRS, DEPARTMENT OF
 Office
-248-NETWORK CONTRACT OFFICE 8 (36C248)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Contract Opportunities
-Current Date Offers Due
-July 29, 2022, 08:00 PM GMT+1
-Notice Type
-Updated Combined Synopsis/Solicitation
-Updated Date
-Jun 7, 2022 (1)
-Published Date
-Jun 7, 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>First Strike Ration</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/698d35418daa4799a8d869b70ffb00bb/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>First Strike Ration
-Notice ID: SPE3S1-22-R-0008
-Solicitation Notice for the upcoming First Strike Ration contract.
+246-NETWORK CONTRACTING OFFICE 6 (36C246)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract Opportunities
+Current Date Offers Due
+July 28, 2022, 03:00 PM GMT+1
+Notice Type
+Original Solicitation
+Updated Date
+Jun 10, 2022
+Published Date
+Jun 10, 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1377-01-448-9910 SS49 GGU-15A/A Gas Generator, Dry Bay Fire Extinguisher</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sam.gov/opp/47ee51aa39094083ba03126a39ea5a0c/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1377-01-448-9910 SS49 GGU-15A/A Gas Generator, Dry Bay Fire Extinguisher
+Notice ID: N0010422RK054
+N772. Paper copies will not be provided. Procurement is restricted to General Dynamics. A limited drawing package is available. Drawings are NOT avail...
+Department/Ind.Agency
+DEPT OF DEFENSE
+Subtier
+DEPT OF THE NAVY
+Office
+NAVSUP WEAPON SYSTEMS SUPPORT MECH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract Opportunities
+Current Date Offers Due
+August 26, 2022, 06:00 AM GMT+1
+Notice Type
+Updated Solicitation
+Updated Date
+Jun 10, 2022 (2)
+Published Date
+Jun 10, 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Marine Corps Wideband Satellite - Light and Heavy (MCWS-L/H) Solicitation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sam.gov/opp/129f69bff51e486ea3151ccf184fd18b/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Marine Corps Wideband Satellite - Light and Heavy (MCWS-L/H) Solicitation
+Notice ID: M6785422R2001
+THIS IS A REQUEST FOR PROPOSAL (RFP). The Marine Corps Systems Command (MCSC), Quantico, VA, requires delivery of Marine Corps Wideband Satellite C
 ...
 Department/Ind.Agency
 DEPT OF DEFENSE
 Subtier
+DEPT OF THE NAVY
+Office
+COMMANDER</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract Opportunities
+Current Date Offers Due
+July 26, 2022, 03:00 PM GMT+1
+Notice Type
+Original Solicitation
+Updated Date
+Jun 10, 2022
+Published Date
+Jun 10, 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gospel Service Worship Leader-Drummer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sam.gov/opp/faaf2120ea124da39061cb697d03f1a6/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gospel Service Worship Leader-Drummer
+Notice ID: W911S7-22-R-0009
+Solicitation, Statement of Work (SOW) and Wage Determination is attached. 
+Questions are due NLT 15 July 2022 by 1600 CST,
+Ans
+...
+Department/Ind.Agency
+DEPT OF DEFENSE
+Subtier
+DEPT OF THE ARMY
+Office
+W6QM MICC-FT LEONARD WOOD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract Opportunities
+Current Date Offers Due
+July 29, 2022, 10:00 PM GMT+1
+Notice Type
+Original Solicitation
+Updated Date
+Jun 10, 2022
+Published Date
+Jun 10, 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Residential Reentry Center (RRC) Services and Home Confinement Services Located in the State of Nebraska within and/or to the West of the Counties of Boyd, Holt, Wheeler, Greeley, Howard, Hall, Hamilton, Clay, or Nuckolls</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sam.gov/opp/c9682e621d5840eebc26a6b14c370018/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Residential Reentry Center (RRC) Services and Home Confinement Services Located in the State of Nebraska within and/or to the West of the Counties of Boyd, Holt, Wheeler, Greeley, Howard, Hall, Hamilton, Clay, or Nuckolls
+Notice ID: 15BRRC22R00000005
+The Federal Bureau of Prisons is seeking concerns having the ability for providing Residential Reentry Center (RRC) services (in-house RRC beds) an
+...
+Department/Ind.Agency
+JUSTICE, DEPARTMENT OF
+Subtier
+FEDERAL PRISON SYSTEM / BUREAU OF PRISONS
+Office
+RESIDENTIAL REENTRY - CO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract Opportunities
+Current Date Offers Due
+August 08, 2022, 07:10 PM GMT+1
+Notice Type
+Original Solicitation
+Updated Date
+Jun 10, 2022
+Published Date
+Jun 10, 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Z1DA--528-19-104 SITE PREP EMERGENCY DEPARTMENT X-RAY EQUIPMENT | Actionable Package: 4/19/2022 l Current Milestone: Presolicitation l Proposed Posting: 5/15/2022 l Proposed Award: 7/15/2022 l Comments: 4/19/2022-Assigned to CO and</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sam.gov/opp/d96d6f0b6b0e43c3b9f0f98449c04150/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Z1DA--528-19-104 SITE PREP EMERGENCY DEPARTMENT X-RAY EQUIPMENT | Actionable Package: 4/19/2022 l Current Milestone: Presolicitation l Proposed Posting: 5/15/2022 l Proposed Award: 7/15/2022 l Comments: 4/19/2022-Assigned to CO and
+Notice ID: 36C24222B0041
+THIS PAGE LEFT BLANK INTENTIONALLY ...
+Department/Ind.Agency
+VETERANS AFFAIRS, DEPARTMENT OF
+Subtier
+VETERANS AFFAIRS, DEPARTMENT OF
+Office
+242-NETWORK CONTRACT OFFICE 02 (36C242)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract Opportunities
+Current Date Offers Due
+July 19, 2022, 06:00 PM GMT+1
+Notice Type
+Updated Solicitation
+Updated Date
+Jun 10, 2022 (1)
+Published Date
+Jun 10, 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WASO_CECH_267542_EX PLAN &amp; DESIGN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sam.gov/opp/d792b8eec4404512900aad0e29d6c959/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WASO_CECH_267542_EX PLAN &amp; DESIGN
+Notice ID: 140P2122R0026
+WASO_CECH_EX PLAN &amp; DESIGN...
+Department/Ind.Agency
+INTERIOR, DEPARTMENT OF THE
+Subtier
+NATIONAL PARK SERVICE
+Office
+WASHINGTON CONTRACTING OFFICE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract Opportunities
+Current Date Offers Due
+July 18, 2022, 03:00 PM GMT+1
+Notice Type
+Original Solicitation
+Updated Date
+Jun 10, 2022
+Published Date
+Jun 10, 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contractor-Owned, Contractor Operated (COCO) Fuel Storage Services on the Island of Oahu, Hawaii</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sam.gov/opp/d710800a165245d994cbe8c36d776ec9/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contractor-Owned, Contractor Operated (COCO) Fuel Storage Services on the Island of Oahu, Hawaii
+Notice ID: SPE603-22-R-0511
+Defense Logistics Agency (DLA) – Energy – FESBB solicitation and attachments for a Contractor-Owned Contractor Operated (COCO) fuel sto
+...
+Department/Ind.Agency
+DEPT OF DEFENSE
+Subtier
 DEFENSE LOGISTICS AGENCY (DLA)
 Office
-DLA TROOP SUPPORT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Contract Opportunities
-Current Date Offers Due
-August 04, 2022, 08:00 PM GMT+1
+DLA ENERGY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract Opportunities
+Current Date Offers Due
+July 25, 2022, 08:00 PM GMT+1
 Notice Type
 Updated Solicitation
 Updated Date
-Jun 7, 2022 (1)
-Published Date
-Jun 7, 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Special Studies, Reporting, and Business Services Support</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/a65b1429760e40ee9e7a63191655dc70/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Special Studies, Reporting, and Business Services Support
-Notice ID: 86614922R00006f
-Special Studies, Reporting, Research, and Business Services Support Basic Purchasing Agreement (BPA). This solicitation is issued under multiple NA
+Jun 10, 2022 (1)
+Published Date
+Jun 10, 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HELICOPTER RESCUE OPS MAINTENANCE HANGAR KADENA AB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sam.gov/opp/e8c9688cb6b44dcfab1bd94c7d385b29/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HELICOPTER RESCUE OPS MAINTENANCE HANGAR KADENA AB
+Notice ID: W912HV22R0005
+June 10, 2022: Extend the proposal due date to 30 August 2022 at 2:00 PM, JST from 14 June 2022. All other terms and condit
 ...
 Department/Ind.Agency
-HOUSING AND URBAN DEVELOPMENT, DEPARTMENT OF
-Subtier
-HOUSING AND URBAN DEVELOPMENT, DEPARTMENT OF
-Office
-CPO : CPO; ACFO; WFCOD; REAL ESTATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Contract Opportunities
-Current Date Offers Due
-July 29, 2022, 06:00 PM GMT+1
-Notice Type
-Original Combined Synopsis/Solicitation
-Updated Date
-Jun 7, 2022
-Published Date
-Jun 7, 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Machine Shop Rapid Prototyping Solicitation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/d37167e22b3b45fb8e019682b6e0445f/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Machine Shop Rapid Prototyping Solicitation
-Notice ID: N0017822R4305
-The Naval Surface Warfare Center, Dahlgren Division (NSWCDD) has a need for the rapid manufacture, assembly, inspection and delivery of machined pr
+DEPT OF DEFENSE
+Subtier
+DEPT OF THE ARMY
+Office
+US ARMY ENGINEER DISTRICT JPN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract Opportunities
+Current Date Offers Due
+August 30, 2022, 06:00 AM GMT+1
+Notice Type
+Updated Solicitation
+Updated Date
+Jun 10, 2022 (3)
+Published Date
+Jun 10, 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Construction: NFSR 700 and 91 Recondition/Resurface</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://sam.gov/opp/8efef603f0264783b79ad0ce1a29c596/view</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Construction: NFSR 700 and 91 Recondition/Resurface
+Notice ID: 127EAX22R0034
+Project:  The USDA Forest Service, Coconino National Forest, Flagstaff Ranger District, has a requirement fo
 ...
 Department/Ind.Agency
-DEPT OF DEFENSE
-Subtier
-DEPT OF THE NAVY
-Office
-NSWC DAHLGREN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Contract Opportunities
-Current Date Offers Due
-July 29, 2022, 05:00 PM GMT+1
-Notice Type
-Updated Solicitation
-Updated Date
-Jun 7, 2022 (2)
-Published Date
-Jun 7, 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/b3fb7959d99c4f368f9f0b708aab436e/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Special Studies, Reporting, and Business Services Support
-Notice ID: 86614922R00006e
-Special Studies, Reporting, Research, and Business Services Support Basic Purchasing Agreement (BPA). This solicitation is issued under multiple NA
-...
-Department/Ind.Agency
-HOUSING AND URBAN DEVELOPMENT, DEPARTMENT OF
-Subtier
-HOUSING AND URBAN DEVELOPMENT, DEPARTMENT OF
-Office
-CPO : CPO; ACFO; WFCOD; REAL ESTATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/3fb601e2aa3c43c9965bfc7227f337d0/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Special Studies, Reporting, and Business Services Support
-Notice ID: 86614922R00006d
-Special Studies, Reporting, Research, and Business Services Support Basic Purchasing Agreement (BPA). This solicitation is issued under multiple NA
-...
-Department/Ind.Agency
-HOUSING AND URBAN DEVELOPMENT, DEPARTMENT OF
-Subtier
-HOUSING AND URBAN DEVELOPMENT, DEPARTMENT OF
-Office
-CPO : CPO; ACFO; WFCOD; REAL ESTATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/ccc9953b3ba340c1847e77840d101934/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Special Studies, Reporting, and Business Services Support
-Notice ID: 86614922R00006c
-Special Studies, Reporting, Research, and Business Services Support Basic Purchasing Agreement (BPA). This solicitation is issued under multiple NA
-...
-Department/Ind.Agency
-HOUSING AND URBAN DEVELOPMENT, DEPARTMENT OF
-Subtier
-HOUSING AND URBAN DEVELOPMENT, DEPARTMENT OF
-Office
-CPO : CPO; ACFO; WFCOD; REAL ESTATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/b81c4ec7623a44229a2ca5a818aee33c/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Special Studies, Reporting, and Business Services Support
-Notice ID: 86614922R00006b
-Special Studies, Reporting, Research, and Business Services Support Basic Purchasing Agreement (BPA). This solicitation is issued under multiple NA
-...
-Department/Ind.Agency
-HOUSING AND URBAN DEVELOPMENT, DEPARTMENT OF
-Subtier
-HOUSING AND URBAN DEVELOPMENT, DEPARTMENT OF
-Office
-CPO : CPO; ACFO; WFCOD; REAL ESTATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/ab5c704200134348b96c988aa4e6ebd8/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Special Studies, Reporting, and Business Services Support
-Notice ID: 86614922R00006a
-Special Studies, Reporting, Research, and Business Services Support Basic Purchasing Agreement (BPA). This solicitation is issued under multiple NA
-...
-Department/Ind.Agency
-HOUSING AND URBAN DEVELOPMENT, DEPARTMENT OF
-Subtier
-HOUSING AND URBAN DEVELOPMENT, DEPARTMENT OF
-Office
-CPO : CPO; ACFO; WFCOD; REAL ESTATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Replace Courtesy Dock, Lake Mead, Nevada</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/b9238855fc744b018e2d5f32709f7731/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Replace Courtesy Dock, Lake Mead, Nevada
-Notice ID: 140P8122R0005
-Replace Courtesy Dock at Hemenway Harbor Lake Mead National Recreation Area...
-Department/Ind.Agency
-INTERIOR, DEPARTMENT OF THE
-Subtier
-NATIONAL PARK SERVICE
-Office
-PWR LAME(81000)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Contract Opportunities
-Current Date Offers Due
-July 21, 2022, 10:00 PM GMT+1
+AGRICULTURE, DEPARTMENT OF
+Subtier
+FOREST SERVICE
+Office
+Southwestern Regional Office, Region 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract Opportunities
+Current Date Offers Due
+July 20, 2022, 12:00 AM GMT+1
 Notice Type
 Original Solicitation
 Updated Date
-Jun 7, 2022
-Published Date
-Jun 7, 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Replace Fishing Pier, Lake Mead, Nevada</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/30cf9f43e10d410b9cbaaccb9ff54f73/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Replace Fishing Pier, Lake Mead, Nevada
-Notice ID: 140P8122R0004
-Replace Hemenway Harbor Fishing Pier, Lake Mead National Recreation Area....
-Department/Ind.Agency
-INTERIOR, DEPARTMENT OF THE
-Subtier
-NATIONAL PARK SERVICE
-Office
-PWR LAME(81000)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stryker Upgrade Kit</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/471b92d98b5f484399484de6e2bf9aae/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stryker Upgrade Kit
-Notice ID: SPRRA2-22-R-0024-0001
-DLA AHCA
-REFER
-June 6, 2022
-Raytheon Company
-2501 W. University Drive,
-McKinney, TX 75071
-RE: Amendment 0001 to
-...
-Department/Ind.Agency
-DEPT OF DEFENSE
-Subtier
-DEFENSE LOGISTICS AGENCY (DLA)
-Office
-DLA AVIATION AT HUNTSVILLE, AL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Contract Opportunities
-Current Date Offers Due
-September 06, 2022, 10:00 PM GMT+1
-Notice Type
-Original Solicitation
-Updated Date
-Jun 7, 2022
-Published Date
-Jun 7, 2022</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mission Planning Support Contract IV (MPSC IV)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://sam.gov/opp/f4f0b6ac52584d5cbc00dcd0216b80dc/view</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mission Planning Support Contract IV (MPSC IV)
-Notice ID: FA8217-22-R-0001
-6/6/2022:
-The purpose of this action is to post the Request for Proposal (RFP) for the Mission Planning Support Contract (MPSC) IV. We are
-...
-Department/Ind.Agency
-DEPT OF DEFENSE
-Subtier
-DEPT OF THE AIR FORCE
-Office
-FA8217 AFLCMC PZZK</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Contract Opportunities
-Current Date Offers Due
-July 21, 2022, 11:00 PM GMT+1
-Notice Type
-Original Solicitation
-Updated Date
-Jun 7, 2022
-Published Date
-Jun 7, 2022</x:t>
+Jun 10, 2022
+Published Date
+Jun 10, 2022</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -710,7 +726,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E15"/>
+  <x:dimension ref="A1:E13"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -805,128 +821,100 @@
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="A7" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
       <x:c r="A8" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="A9" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
       <x:c r="A10" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
       <x:c r="A11" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
       <x:c r="A12" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="A13" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:5">
-      <x:c r="A14" s="0" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="B14" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C14" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:5">
-      <x:c r="A15" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="C15" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="D15" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>